<commit_message>
added header=False on excel output. Files upload to A2
</commit_message>
<xml_diff>
--- a/test_R186_ext_spot.xlsx
+++ b/test_R186_ext_spot.xlsx
@@ -12,6 +12,9 @@
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,65 +376,61 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Key</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
+          <t>specificType</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>rsaBond</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>specificType</t>
+          <t>contractSubType</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>rsaBond</t>
+          <t>RSA Bond{token}RSA Bond</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>contractSubType</t>
+          <t>tradeReference</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RSA Bond{token}RSA Bond</t>
+          <t>R186</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>tradeReference</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R186</t>
-        </is>
+          <t>transactionDate</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>43934.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>transactionDate</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>43934.5</v>
-      </c>
+          <t>reissuedDate</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>reissuedDate</t>
+          <t>reissuedReference</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -439,115 +438,115 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>reissuedReference</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr"/>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>A:LG:ALM MRM ANN AND GCB:GOVBND:U</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>book</t>
+          <t>counterparty</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>A:LG:ALM MRM ANN AND GCB:GOVBND:U</t>
+          <t>Government of South Africa|Global Markets Liberty</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>counterparty</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Government of South Africa|Global Markets Liberty</t>
-        </is>
+          <t>numberOfUnits</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>numberOfUnits</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>100</v>
+          <t>specialInfo1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SBSA</t>
+        </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>specialInfo1</t>
+          <t>specialInfo2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SBSA</t>
+          <t>Jacob</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>specialInfo2</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Jacob</t>
-        </is>
+          <t>collateralInfoType</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>collateralInfoType</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
+          <t>fundingStatus</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Unfunded</t>
+        </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>fundingStatus</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Unfunded</t>
-        </is>
-      </c>
+          <t>workflowReference</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>workflowReference</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr"/>
+          <t>riskDefinition</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>TRADING</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>riskDefinition</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>TRADING</t>
-        </is>
-      </c>
+          <t>externalReference</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>externalReference</t>
+          <t>csa</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -555,7 +554,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>csa</t>
+          <t>dataExportInfo</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -563,84 +562,76 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>dataExportInfo</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr"/>
+          <t>bond</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>R186</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>bond</t>
+          <t>referenceIndex</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>R186</t>
+          <t>Bond</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>referenceIndex</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Bond</t>
-        </is>
+          <t>notionalAmount</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1000000</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>notionalAmount</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>1000000</v>
+          <t>bondPricingType</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Yield</t>
+        </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>bondPricingType</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Yield</t>
-        </is>
+          <t>tradeYieldOrPrice</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>tradeYieldOrPrice</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0.1</v>
+          <t>nonStandardSettlement</t>
+        </is>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>nonStandardSettlement</t>
-        </is>
-      </c>
-      <c r="B25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
           <t>nonStandardSettlementLag</t>
         </is>
       </c>
-      <c r="B26" t="n">
+      <c r="B25" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>